<commit_message>
Add lab 6, lab 8, and project 3
</commit_message>
<xml_diff>
--- a/Project3/Experiments.xlsx
+++ b/Project3/Experiments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t xml:space="preserve">Start Node </t>
   </si>
@@ -150,6 +150,15 @@
   </si>
   <si>
     <t>pref = 2 longest site</t>
+  </si>
+  <si>
+    <t>181 131 63 100 26 4 57 181 </t>
+  </si>
+  <si>
+    <t>179 190 165 </t>
+  </si>
+  <si>
+    <t>181 179 190 165 66 181 </t>
   </si>
 </sst>
 </file>
@@ -192,7 +201,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -200,11 +209,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -212,22 +236,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,455 +536,475 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" style="2" customWidth="1"/>
     <col min="2" max="3" width="10.83203125" style="2"/>
-    <col min="4" max="4" width="20.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="13.1640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="2"/>
-    <col min="7" max="7" width="34" style="2" customWidth="1"/>
+    <col min="7" max="7" width="22.5" style="2" customWidth="1"/>
     <col min="8" max="8" width="61.1640625" style="2" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3"/>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="5"/>
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="10" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
-        <v>130</v>
-      </c>
-      <c r="C2" s="3">
+      <c r="B2" s="5">
+        <v>130</v>
+      </c>
+      <c r="C2" s="5">
         <v>50</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="5">
         <v>29</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="5">
         <v>25</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="6">
         <v>103</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
-        <v>130</v>
-      </c>
-      <c r="C3" s="3">
+      <c r="B3" s="5">
+        <v>130</v>
+      </c>
+      <c r="C3" s="5">
         <v>100</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="5">
         <v>100</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="5">
         <v>89</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
-        <v>130</v>
-      </c>
-      <c r="C4" s="3">
+      <c r="B4" s="5">
+        <v>130</v>
+      </c>
+      <c r="C4" s="5">
         <v>150</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="5">
         <v>159</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="5">
         <v>139</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
-        <v>130</v>
-      </c>
-      <c r="C5" s="3">
+      <c r="B5" s="5">
+        <v>130</v>
+      </c>
+      <c r="C5" s="5">
         <v>500</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="5">
         <v>336</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="5">
         <v>331</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
-        <v>130</v>
-      </c>
-      <c r="C6" s="3">
+      <c r="B6" s="5">
+        <v>130</v>
+      </c>
+      <c r="C6" s="5">
         <v>50</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="6">
         <v>157</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="5">
         <v>39</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="5">
         <v>29</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
-        <v>130</v>
-      </c>
-      <c r="C7" s="3">
+      <c r="B7" s="5">
+        <v>130</v>
+      </c>
+      <c r="C7" s="5">
         <v>100</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="6">
         <v>157</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="5">
         <v>89</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="5">
         <v>79</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="3">
-        <v>130</v>
-      </c>
-      <c r="C8" s="3">
+      <c r="B8" s="5">
+        <v>130</v>
+      </c>
+      <c r="C8" s="5">
         <v>150</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="5">
         <v>109</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="5">
         <v>98</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="3">
-        <v>130</v>
-      </c>
-      <c r="C9" s="3">
+      <c r="B9" s="5">
+        <v>130</v>
+      </c>
+      <c r="C9" s="5">
         <v>150</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="5">
         <v>111</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="5">
         <v>98</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="3">
-        <v>130</v>
-      </c>
-      <c r="C10" s="3">
+      <c r="B10" s="5">
+        <v>130</v>
+      </c>
+      <c r="C10" s="5">
         <v>100</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="5">
         <v>75</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="5">
         <v>70</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="3">
-        <v>130</v>
-      </c>
-      <c r="C11" s="3">
+      <c r="B11" s="5">
+        <v>130</v>
+      </c>
+      <c r="C11" s="5">
         <v>100</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="5">
         <v>80</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="5">
         <v>71</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="3">
-        <v>130</v>
-      </c>
-      <c r="C12" s="3">
+      <c r="B12" s="5">
+        <v>130</v>
+      </c>
+      <c r="C12" s="5">
         <v>150</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="9">
         <v>134</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="5">
         <v>121</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" s="3">
-        <v>130</v>
-      </c>
-      <c r="C13" s="3">
+      <c r="B13" s="5">
+        <v>130</v>
+      </c>
+      <c r="C13" s="5">
         <v>150</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="5">
         <v>121</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="5">
         <v>111</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="8" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
+      <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="B14" s="5">
+        <v>181</v>
+      </c>
+      <c r="C14" s="5">
+        <v>50</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="5">
+        <v>35</v>
+      </c>
+      <c r="F14" s="5">
+        <v>29</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="5">
         <v>181</v>
       </c>
-      <c r="C15" s="3">
-        <v>50</v>
-      </c>
-      <c r="D15" s="3" t="s">
+      <c r="C15" s="5">
+        <v>100</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="3">
-        <v>35</v>
-      </c>
-      <c r="F15" s="3">
+      <c r="E15" s="5">
+        <v>88</v>
+      </c>
+      <c r="F15" s="5">
+        <v>79</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5">
+        <v>181</v>
+      </c>
+      <c r="C16" s="5">
+        <v>100</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="5">
+        <v>77</v>
+      </c>
+      <c r="F16" s="5">
+        <v>70</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5">
+        <v>181</v>
+      </c>
+      <c r="C17" s="5">
+        <v>100</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
-        <v>15</v>
-      </c>
-      <c r="B16" s="3">
-        <v>181</v>
-      </c>
-      <c r="C16" s="3">
-        <v>100</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
-        <v>16</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
-        <v>17</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+      <c r="E17" s="5">
+        <v>99</v>
+      </c>
+      <c r="F17" s="5">
+        <v>90</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>